<commit_message>
hoangtri done bai-19 dataprovider with excel
</commit_message>
<xml_diff>
--- a/src/test/resources/suites/testdata/TestData.xlsx
+++ b/src/test/resources/suites/testdata/TestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Testcase ID</t>
   </si>
@@ -668,13 +668,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="13.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="32.85546875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="11" width="12.42578125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="11" width="19.42578125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="44.0" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="38.5703125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="12.5703125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="32.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="11" width="12.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="11" width="19.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="44.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="38.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -711,7 +711,9 @@
         <v>38</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -829,11 +831,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="16.5703125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="27.85546875" collapsed="false"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="8" width="41.7109375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="13.7109375" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="41.85546875" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="16.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="27.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="8" width="41.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="41.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>